<commit_message>
updated code for dynamic xml creator and dynamic class creator
</commit_message>
<xml_diff>
--- a/ProjectAutomationFiles/testcases/Client_TestSuite.xlsx
+++ b/ProjectAutomationFiles/testcases/Client_TestSuite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>TestcaseType</t>
   </si>
@@ -38,45 +38,6 @@
     <t>Smoke</t>
   </si>
   <si>
-    <t>Given User is on SSP adviser portal</t>
-  </si>
-  <si>
-    <t>Comman_Reusables.launchAdviser</t>
-  </si>
-  <si>
-    <t>WhenUser logs in with valid credentials</t>
-  </si>
-  <si>
-    <t>login_Page.loginWithUser</t>
-  </si>
-  <si>
-    <t>Login_Testdata|Login_Credentials|1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Then User should be able to login </t>
-  </si>
-  <si>
-    <t>Home_Page.validate_UserIsLoggedIn</t>
-  </si>
-  <si>
-    <t>Personal Client Creation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When User is on "Personal Client" creation page </t>
-  </si>
-  <si>
-    <t xml:space="preserve">And User creates the personal client with mandatory valid details </t>
-  </si>
-  <si>
-    <t>Home_Page.openPersonalClientCreationPage</t>
-  </si>
-  <si>
-    <t>Client_Page.personalClientCreationPageDisplayed</t>
-  </si>
-  <si>
-    <t>URL_testdata|URLs|1</t>
-  </si>
-  <si>
     <t>Client_Page.createPersonalClient</t>
   </si>
   <si>
@@ -86,13 +47,46 @@
     <t>Client_Page.clickSaveButtonOnSummaryPage</t>
   </si>
   <si>
-    <t>Client_Page.personalClientCreationTitleDisplayed</t>
-  </si>
-  <si>
-    <t>Comman_Reusables.closeBrowser</t>
-  </si>
-  <si>
     <t>Client.001</t>
+  </si>
+  <si>
+    <t>User is on way2automationHomePage</t>
+  </si>
+  <si>
+    <t>Comman_Reusables.launchURL</t>
+  </si>
+  <si>
+    <t>Home_Page.validateUserIsOnHomePage</t>
+  </si>
+  <si>
+    <t>User clicks on the registration link</t>
+  </si>
+  <si>
+    <t>Home_Page.clickRegistrationLink</t>
+  </si>
+  <si>
+    <t>Registration pop up is displayed</t>
+  </si>
+  <si>
+    <t>Home_Page.validateRegistrationFormDisplayed</t>
+  </si>
+  <si>
+    <t>Register with a valid user</t>
+  </si>
+  <si>
+    <t>home_Page.registrationOnPopUp</t>
+  </si>
+  <si>
+    <t>Registration_testdata|Registration_Details|1</t>
+  </si>
+  <si>
+    <t>Registration_Page.registrationOnRegistrationPage</t>
+  </si>
+  <si>
+    <t>Registration_testdata|Registration_Details|1-2</t>
+  </si>
+  <si>
+    <t>Client First Test Case</t>
   </si>
 </sst>
 </file>
@@ -443,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -484,64 +478,56 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -561,15 +547,15 @@
   <sheetData>
     <row r="13" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F13" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>